<commit_message>
try-outs Svetlana and feedback
-Folder for code txts
-New data files
-Documents folder (instructions, grids)
-Embedding of Svetlana's feedback on famil.session and main task.
</commit_message>
<xml_diff>
--- a/repswitch.xlsx
+++ b/repswitch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3F410B-4D0A-4F06-8A36-75E01B75F85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18424E86-40DF-49C1-9A5A-EB238F40F2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11508" yWindow="600" windowWidth="11532" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18288" yWindow="708" windowWidth="7764" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="9" r:id="rId1"/>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE5FFB8-ADEE-4233-9EF1-4711A9BB639D}">
   <dimension ref="A1:I385"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>